<commit_message>
Back to the meta-analysis!
</commit_message>
<xml_diff>
--- a/Meta_analysis/Metaanalysis_ArticleSelection.xlsx
+++ b/Meta_analysis/Metaanalysis_ArticleSelection.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7872" uniqueCount="3226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7873" uniqueCount="3226">
   <si>
     <t>NA</t>
   </si>
@@ -9612,13 +9612,7 @@
     <t>NMDS without coordinates.</t>
   </si>
   <si>
-    <t>PCoA with just 3 points per site, alpha diversity indexes = mean +/- WHAT (they do not specify if SE or SD, we asumed SE)</t>
-  </si>
-  <si>
     <t>As BURNED treatment I have chosen just B1 because: a) it was the short-interval (more severe effects) and it was covered by Cistus ladanifer (ECM) after the fire. CA_quercus_B1 has only 3 points??</t>
-  </si>
-  <si>
-    <t>We have only included pyrosequencing data since DGGE did not present SD values in most cases</t>
   </si>
   <si>
     <t>We only kept info from NON-AUTOCLAVED</t>
@@ -9681,9 +9675,6 @@
     <t>Only 2 points in the DCA for the 4-year burnt treatment: is not possible to calculate the variance</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>DNA results EXCLUDED because of no variation measures. ONLY SPOROCARP SURVEY</t>
   </si>
   <si>
@@ -9709,6 +9700,15 @@
   </si>
   <si>
     <t>NO_REPLICATES</t>
+  </si>
+  <si>
+    <t>We have only included pyrosequencing data since DGGE did not present SD values in most cases. We've retained CHAO1 since no richness is provided</t>
+  </si>
+  <si>
+    <t>PCoA with just 3 points per site, alpha diversity indexes = mean +/- WHAT (they do not specify if SE or SD, we asumed SE). We've retained CHAO1 since no richness is provided</t>
+  </si>
+  <si>
+    <t>We've retained CHAO1 since no richness is provided</t>
   </si>
 </sst>
 </file>
@@ -10195,7 +10195,7 @@
   <dimension ref="A1:Y1056"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R381" sqref="R381"/>
+      <selection activeCell="A403" sqref="A403:XFD403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11370,10 +11370,10 @@
         <v>1</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11665,7 +11665,7 @@
         <v>1</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="31" spans="1:21" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -11911,7 +11911,7 @@
         <v>1</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S35" s="3" t="s">
         <v>3035</v>
@@ -11966,7 +11966,7 @@
         <v>11</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>3214</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -12316,7 +12316,7 @@
         <v>1</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -12370,7 +12370,7 @@
         <v>1</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="45" spans="1:19" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -12467,7 +12467,7 @@
         <v>11</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>3200</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="47" spans="1:19" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -12714,7 +12714,7 @@
         <v>11</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>3215</v>
+        <v>3213</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -12768,7 +12768,7 @@
         <v>1</v>
       </c>
       <c r="R52" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13597,7 +13597,7 @@
         <v>11</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>3199</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13706,7 +13706,7 @@
         <v>1</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13855,7 +13855,7 @@
         <v>11</v>
       </c>
       <c r="S74" s="22" t="s">
-        <v>3198</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -14460,13 +14460,13 @@
       </c>
       <c r="P86" s="8"/>
       <c r="Q86" s="8" t="s">
-        <v>3216</v>
+        <v>1</v>
       </c>
       <c r="R86" s="19" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="S86" s="19" t="s">
-        <v>3197</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="87" spans="1:25" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -14719,7 +14719,7 @@
         <v>11</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>3196</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="92" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14771,7 +14771,7 @@
         <v>11</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>3195</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="93" spans="1:25" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -14880,7 +14880,7 @@
         <v>1</v>
       </c>
       <c r="R94" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="T94" s="3"/>
       <c r="U94" s="3"/>
@@ -15378,7 +15378,7 @@
         <v>1</v>
       </c>
       <c r="R104" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="105" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -15579,7 +15579,7 @@
         <v>11</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>3194</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="109" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -15679,7 +15679,7 @@
         <v>1</v>
       </c>
       <c r="R110" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="S110" s="3" t="s">
         <v>2681</v>
@@ -16229,7 +16229,7 @@
         <v>1</v>
       </c>
       <c r="R121" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="122" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -16283,7 +16283,7 @@
         <v>1</v>
       </c>
       <c r="R122" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="123" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16435,7 +16435,7 @@
         <v>1</v>
       </c>
       <c r="R125" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="126" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -16487,7 +16487,7 @@
         <v>1</v>
       </c>
       <c r="R126" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S126" s="3" t="s">
         <v>2605</v>
@@ -16838,7 +16838,7 @@
         <v>1</v>
       </c>
       <c r="R133" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="134" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -16938,7 +16938,7 @@
         <v>11</v>
       </c>
       <c r="S135" s="3" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="136" spans="1:19" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -17289,7 +17289,7 @@
         <v>1</v>
       </c>
       <c r="R142" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="143" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -17390,10 +17390,10 @@
         <v>1</v>
       </c>
       <c r="R144" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="S144" s="22" t="s">
-        <v>3209</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="145" spans="1:19" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -17644,7 +17644,7 @@
         <v>1</v>
       </c>
       <c r="R149" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S149" s="3" t="s">
         <v>2498</v>
@@ -18442,7 +18442,7 @@
         <v>1</v>
       </c>
       <c r="R165" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="166" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -19094,7 +19094,7 @@
         <v>1</v>
       </c>
       <c r="R178" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="179" spans="1:19" s="7" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -19197,7 +19197,7 @@
         <v>11</v>
       </c>
       <c r="S180" s="3" t="s">
-        <v>3218</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="181" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -19496,7 +19496,7 @@
         <v>1</v>
       </c>
       <c r="R186" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="187" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -19650,7 +19650,7 @@
         <v>1</v>
       </c>
       <c r="R189" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="190" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19750,7 +19750,7 @@
       </c>
       <c r="P191" s="29"/>
     </row>
-    <row r="192" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>111</v>
       </c>
@@ -19796,7 +19796,7 @@
       </c>
       <c r="P192" s="4"/>
       <c r="Q192" s="2" t="s">
-        <v>3216</v>
+        <v>11</v>
       </c>
       <c r="S192" s="3" t="s">
         <v>3191</v>
@@ -20455,7 +20455,7 @@
         <v>1</v>
       </c>
       <c r="R205" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="206" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -21938,7 +21938,7 @@
         <v>1</v>
       </c>
       <c r="R235" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="S235" s="19"/>
     </row>
@@ -22341,7 +22341,7 @@
         <v>1</v>
       </c>
       <c r="R243" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="244" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -22395,7 +22395,7 @@
         <v>1</v>
       </c>
       <c r="R244" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="245" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -22498,7 +22498,7 @@
         <v>3170</v>
       </c>
       <c r="S246" s="3" t="s">
-        <v>3205</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="247" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -22653,7 +22653,7 @@
         <v>1</v>
       </c>
       <c r="R249" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="250" spans="1:19" s="3" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -24560,7 +24560,7 @@
         <v>1</v>
       </c>
       <c r="R287" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="288" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -24612,7 +24612,7 @@
         <v>1</v>
       </c>
       <c r="R288" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="289" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -25196,7 +25196,7 @@
         <v>1</v>
       </c>
       <c r="R300" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S300" s="3" t="s">
         <v>1769</v>
@@ -25548,7 +25548,7 @@
         <v>1</v>
       </c>
       <c r="R307" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S307" s="3" t="s">
         <v>707</v>
@@ -25603,7 +25603,7 @@
         <v>1</v>
       </c>
       <c r="R308" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="309" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -25707,7 +25707,7 @@
         <v>11</v>
       </c>
       <c r="S310" s="3" t="s">
-        <v>3219</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="311" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -26090,7 +26090,7 @@
         <v>1</v>
       </c>
       <c r="R318" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S318" s="3" t="s">
         <v>1667</v>
@@ -26241,7 +26241,7 @@
         <v>11</v>
       </c>
       <c r="S321" s="3" t="s">
-        <v>3220</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="322" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -26634,7 +26634,7 @@
       </c>
       <c r="R329" s="19"/>
       <c r="S329" s="19" t="s">
-        <v>3210</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="330" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -27483,6 +27483,9 @@
       <c r="Q346" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="S346" s="3" t="s">
+        <v>3225</v>
+      </c>
     </row>
     <row r="347" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="3">
@@ -27862,7 +27865,7 @@
         <v>1</v>
       </c>
       <c r="R354" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S354" s="3" t="s">
         <v>1487</v>
@@ -28358,10 +28361,10 @@
         <v>1</v>
       </c>
       <c r="R364" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="S364" s="3" t="s">
-        <v>3221</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="365" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -28509,13 +28512,13 @@
       </c>
       <c r="P367" s="4"/>
       <c r="Q367" s="2" t="s">
-        <v>3216</v>
+        <v>1</v>
       </c>
       <c r="R367" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="S367" s="3" t="s">
-        <v>3222</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="368" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -29122,7 +29125,7 @@
         <v>82</v>
       </c>
       <c r="R379" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="380" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -29174,7 +29177,7 @@
         <v>1</v>
       </c>
       <c r="R380" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S380" s="3" t="s">
         <v>3177</v>
@@ -29337,7 +29340,7 @@
         <v>1</v>
       </c>
       <c r="R383" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="384" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -29906,7 +29909,7 @@
         <v>1</v>
       </c>
       <c r="R394" s="3" t="s">
-        <v>3225</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="395" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30348,7 +30351,7 @@
         <v>11</v>
       </c>
       <c r="S403" s="3" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="404" spans="1:24" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -30400,7 +30403,7 @@
         <v>1</v>
       </c>
       <c r="R404" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S404" s="3" t="s">
         <v>1225</v>
@@ -30796,7 +30799,7 @@
         <v>1</v>
       </c>
       <c r="R412" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S412" s="3" t="s">
         <v>1186</v>
@@ -30900,7 +30903,7 @@
         <v>1</v>
       </c>
       <c r="R414" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="415" spans="1:24" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -31695,7 +31698,7 @@
         <v>1</v>
       </c>
       <c r="R430" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="431" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -32941,7 +32944,7 @@
         <v>1</v>
       </c>
       <c r="R455" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S455" s="3" t="s">
         <v>967</v>
@@ -33187,7 +33190,7 @@
         <v>1</v>
       </c>
       <c r="R460" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="461" spans="1:19" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -33386,7 +33389,7 @@
         <v>1</v>
       </c>
       <c r="R464" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="465" spans="1:19" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -33538,7 +33541,7 @@
         <v>1</v>
       </c>
       <c r="R467" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="468" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -33939,7 +33942,7 @@
         <v>1</v>
       </c>
       <c r="R475" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="476" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34244,7 +34247,7 @@
         <v>1</v>
       </c>
       <c r="R481" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="S481" s="19"/>
     </row>
@@ -34643,7 +34646,7 @@
         <v>1</v>
       </c>
       <c r="R489" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S489" s="3" t="s">
         <v>707</v>
@@ -34698,7 +34701,7 @@
         <v>1</v>
       </c>
       <c r="R490" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="491" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34853,7 +34856,7 @@
         <v>11</v>
       </c>
       <c r="S493" s="3" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="494" spans="1:19" s="7" customFormat="1" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
@@ -35046,7 +35049,7 @@
         <v>1</v>
       </c>
       <c r="R497" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="S497" s="19"/>
     </row>
@@ -35097,7 +35100,7 @@
         <v>1</v>
       </c>
       <c r="R498" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="499" spans="1:19" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -35489,7 +35492,7 @@
         <v>1</v>
       </c>
       <c r="R506" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S506" s="3" t="s">
         <v>707</v>
@@ -35843,7 +35846,7 @@
         <v>1</v>
       </c>
       <c r="R513" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="514" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36032,7 +36035,7 @@
         <v>1</v>
       </c>
       <c r="R517" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="518" spans="1:19" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -36701,7 +36704,7 @@
         <v>1</v>
       </c>
       <c r="R530" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="531" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37388,7 +37391,7 @@
         <v>1</v>
       </c>
       <c r="R544" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="545" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37681,7 +37684,7 @@
         <v>1</v>
       </c>
       <c r="R550" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="S550" s="19"/>
     </row>
@@ -37931,7 +37934,7 @@
         <v>1</v>
       </c>
       <c r="R555" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="556" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -38439,7 +38442,7 @@
         <v>1</v>
       </c>
       <c r="R565" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="566" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -38493,7 +38496,7 @@
         <v>1</v>
       </c>
       <c r="R566" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="567" spans="1:19" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -38699,7 +38702,7 @@
         <v>150</v>
       </c>
       <c r="S570" s="3" t="s">
-        <v>3202</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="571" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -38902,10 +38905,10 @@
         <v>351</v>
       </c>
       <c r="C575" s="25" t="s">
-        <v>3203</v>
+        <v>3201</v>
       </c>
       <c r="D575" s="26" t="s">
-        <v>3204</v>
+        <v>3202</v>
       </c>
       <c r="E575" s="26"/>
       <c r="F575" s="26"/>
@@ -38930,7 +38933,7 @@
         <v>150</v>
       </c>
       <c r="S575" s="3" t="s">
-        <v>3202</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="576" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -39037,7 +39040,7 @@
         <v>1</v>
       </c>
       <c r="R577" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S577" s="3" t="s">
         <v>319</v>
@@ -39140,7 +39143,7 @@
         <v>1</v>
       </c>
       <c r="R579" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S579" s="3" t="s">
         <v>305</v>
@@ -39343,7 +39346,7 @@
         <v>1</v>
       </c>
       <c r="R583" s="3" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="584" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -39444,7 +39447,7 @@
         <v>1</v>
       </c>
       <c r="R585" s="3" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="S585" s="3" t="s">
         <v>269</v>
@@ -40061,7 +40064,7 @@
         <v>1</v>
       </c>
       <c r="R597" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="598" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -41012,7 +41015,7 @@
         <v>1</v>
       </c>
       <c r="R616" s="3" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="617" spans="1:19" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -41700,19 +41703,19 @@
     </row>
     <row r="634" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C634" s="31" t="s">
-        <v>3207</v>
+        <v>3205</v>
       </c>
       <c r="Q634" s="3"/>
     </row>
     <row r="635" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C635" s="20" t="s">
-        <v>3208</v>
+        <v>3206</v>
       </c>
       <c r="Q635" s="3"/>
     </row>
     <row r="636" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C636" s="30" t="s">
-        <v>3206</v>
+        <v>3204</v>
       </c>
       <c r="Q636" s="3"/>
     </row>
@@ -42966,11 +42969,6 @@
     <row r="1056" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A1:X632">
-    <filterColumn colId="10">
-      <filters blank="1">
-        <filter val="YES"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="16">
       <filters>
         <filter val="YES"/>

</xml_diff>